<commit_message>
Auto-committed on 2021/12/15 週三
Former-commit-id: 47991f8f9fba498c1efee8e3f388d69f9704547f
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/CdSyndFee.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/CdSyndFee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L6-共同作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE2991B-D5C2-4374-BB1B-A2315F5B45D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE955F7-5BF7-4C93-9BF3-E2302CD0719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -910,7 +910,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>

</xml_diff>